<commit_message>
Added add/delete/update metadata, bond conditions and surety
</commit_message>
<xml_diff>
--- a/schemas/CaseUpdates_iepd/artifacts/CaseInitiation_MappingSpreasheet - Case Updates.xlsx
+++ b/schemas/CaseUpdates_iepd/artifacts/CaseInitiation_MappingSpreasheet - Case Updates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\CaseUpdates_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68148510-8F0D-4DFD-BEB7-F861F93FAD9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBC3AB4-C95D-4C56-B6BB-C493AF06CDB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4065" yWindow="-21600" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Case Initiation" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1852" uniqueCount="911">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1864" uniqueCount="920">
   <si>
     <t/>
   </si>
@@ -2326,9 +2326,6 @@
     <t>/j:CaseCharge/hs:ChargeAugmentation/j:BailBond/nola-ext:BailBondAugmentation/nola-ext:EnhancedBond</t>
   </si>
   <si>
-    <t>/nola:CaseInitiationExchange/CourtCase/j:CaseAugmentation/j:CaseCharge/hs:ChargeAugmentation/j:BailBond/nola-ext:BailBondAugmentation/nola-ext:EnhancedBond</t>
-  </si>
-  <si>
     <t>[{"db": "AS400_CDC_CMS",	"table": "BNDHST",	"fieldDesc": "NoBondFlag",	"field": "BHNONE"},
 {"db": "MC",	"table": "DigiCourt_Orleans.dbview.vw_AllWarrants",	"fieldDesc": "HoldwithoutBond",	"field": "HOLD_WITHOUT_BOND"}]</t>
   </si>
@@ -3292,6 +3289,36 @@
   </si>
   <si>
     <t>Bondsman or bonding company</t>
+  </si>
+  <si>
+    <t>/j:BailBond/j:BailBondConditionDescriptionText</t>
+  </si>
+  <si>
+    <t>/nola:CaseInitiationExchange/CourtCase/j:CaseAugmentation/j:CaseCharge/hs:ChargeAugmentation/j:BailBond/j:BailBondConditionDescriptionText</t>
+  </si>
+  <si>
+    <t>/j:BailBond/j:BailBondSuretyEntity</t>
+  </si>
+  <si>
+    <t>/nola:CaseInitiationExchange/CourtCase/j:CaseAugmentation/j:CaseCharge/hs:ChargeAugmentation/j:BailBond/j:BailBondSuretyEntity</t>
+  </si>
+  <si>
+    <t>j:BailBondConditionDescriptionText</t>
+  </si>
+  <si>
+    <t>j:BailBondSuretyEntity</t>
+  </si>
+  <si>
+    <t>structures:MetadataType</t>
+  </si>
+  <si>
+    <t>/nola-ext:UpdateType</t>
+  </si>
+  <si>
+    <t>nola-ext:MessageUpdateCode</t>
+  </si>
+  <si>
+    <t>nola-ext:UpdateCode</t>
   </si>
 </sst>
 </file>
@@ -3320,7 +3347,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3350,8 +3377,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -3411,11 +3444,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3454,6 +3511,24 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4002,8 +4077,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C1555FB-E16C-423D-A1FA-98AD99C9E15B}" name="MappingSpreadsheet" displayName="MappingSpreadsheet" ref="A1:O148" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
-  <autoFilter ref="A1:O148" xr:uid="{2C1555FB-E16C-423D-A1FA-98AD99C9E15B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C1555FB-E16C-423D-A1FA-98AD99C9E15B}" name="MappingSpreadsheet" displayName="MappingSpreadsheet" ref="A1:O149" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+  <autoFilter ref="A1:O149" xr:uid="{2C1555FB-E16C-423D-A1FA-98AD99C9E15B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O148">
     <sortCondition ref="C1:C148"/>
   </sortState>
@@ -4325,13 +4400,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O148"/>
+  <dimension ref="A1:O149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="K143" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomRight" activeCell="N149" sqref="N149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -4346,19 +4421,19 @@
     <col min="8" max="8" width="13.19921875" customWidth="1"/>
     <col min="10" max="10" width="126.33203125" customWidth="1"/>
     <col min="11" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="15.1328125" customWidth="1"/>
+    <col min="14" max="14" width="20.53125" customWidth="1"/>
     <col min="15" max="15" width="12.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>8</v>
@@ -4411,7 +4486,7 @@
         <v>226</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="4" t="s">
@@ -4832,7 +4907,7 @@
         <v>690</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -4845,24 +4920,32 @@
         <v>226</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>14</v>
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
+      <c r="K12" s="14" t="s">
+        <v>914</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>461</v>
+      </c>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14" t="s">
+        <v>910</v>
+      </c>
+      <c r="O12" s="14" t="s">
+        <v>911</v>
+      </c>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="12"/>
@@ -4874,24 +4957,32 @@
         <v>226</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>14</v>
       </c>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
+      <c r="K13" s="14" t="s">
+        <v>915</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>538</v>
+      </c>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14" t="s">
+        <v>912</v>
+      </c>
+      <c r="O13" s="14" t="s">
+        <v>913</v>
+      </c>
     </row>
     <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="7" t="s">
@@ -4922,20 +5013,20 @@
         <v>258</v>
       </c>
       <c r="J14" s="9" t="s">
+        <v>691</v>
+      </c>
+      <c r="K14" s="9" t="s">
         <v>692</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>693</v>
       </c>
       <c r="L14" s="9" t="s">
         <v>604</v>
       </c>
       <c r="M14" s="9"/>
       <c r="N14" s="9" t="s">
+        <v>693</v>
+      </c>
+      <c r="O14" s="9" t="s">
         <v>694</v>
-      </c>
-      <c r="O14" s="9" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -4952,7 +5043,7 @@
         <v>10</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="4" t="s">
@@ -5075,7 +5166,7 @@
         <v>288</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="4" t="s">
@@ -5125,10 +5216,10 @@
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
       <c r="N19" s="9" t="s">
+        <v>886</v>
+      </c>
+      <c r="O19" s="9" t="s">
         <v>887</v>
-      </c>
-      <c r="O19" s="9" t="s">
-        <v>888</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5160,20 +5251,20 @@
         <v>291</v>
       </c>
       <c r="J20" s="9" t="s">
+        <v>727</v>
+      </c>
+      <c r="K20" s="9" t="s">
         <v>728</v>
-      </c>
-      <c r="K20" s="9" t="s">
-        <v>729</v>
       </c>
       <c r="L20" s="9" t="s">
         <v>456</v>
       </c>
       <c r="M20" s="9"/>
       <c r="N20" s="9" t="s">
+        <v>729</v>
+      </c>
+      <c r="O20" s="9" t="s">
         <v>730</v>
-      </c>
-      <c r="O20" s="9" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5205,7 +5296,7 @@
         <v>294</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="K21" s="9" t="s">
         <v>455</v>
@@ -5215,10 +5306,10 @@
       </c>
       <c r="M21" s="9"/>
       <c r="N21" s="9" t="s">
+        <v>732</v>
+      </c>
+      <c r="O21" s="9" t="s">
         <v>733</v>
-      </c>
-      <c r="O21" s="9" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5229,13 +5320,13 @@
         <v>260</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>261</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="4" t="s">
@@ -5247,14 +5338,14 @@
       </c>
       <c r="J22" s="4"/>
       <c r="K22" s="4" t="s">
+        <v>695</v>
+      </c>
+      <c r="L22" s="4" t="s">
         <v>696</v>
-      </c>
-      <c r="L22" s="4" t="s">
-        <v>697</v>
       </c>
       <c r="M22" s="4"/>
       <c r="N22" s="4" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="O22" s="4"/>
     </row>
@@ -5266,7 +5357,7 @@
         <v>266</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>261</v>
@@ -5287,20 +5378,20 @@
         <v>267</v>
       </c>
       <c r="J23" s="9" t="s">
+        <v>701</v>
+      </c>
+      <c r="K23" s="9" t="s">
         <v>702</v>
-      </c>
-      <c r="K23" s="9" t="s">
-        <v>703</v>
       </c>
       <c r="L23" s="9" t="s">
         <v>477</v>
       </c>
       <c r="M23" s="9"/>
       <c r="N23" s="9" t="s">
+        <v>703</v>
+      </c>
+      <c r="O23" s="9" t="s">
         <v>704</v>
-      </c>
-      <c r="O23" s="9" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5311,7 +5402,7 @@
         <v>263</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>261</v>
@@ -5333,10 +5424,10 @@
       </c>
       <c r="J24" s="9"/>
       <c r="K24" s="9" t="s">
+        <v>698</v>
+      </c>
+      <c r="L24" s="9" t="s">
         <v>699</v>
-      </c>
-      <c r="L24" s="9" t="s">
-        <v>700</v>
       </c>
       <c r="M24" s="9" t="s">
         <v>0</v>
@@ -5345,7 +5436,7 @@
         <v>0</v>
       </c>
       <c r="O24" s="9" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5356,7 +5447,7 @@
         <v>269</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>261</v>
@@ -5377,20 +5468,20 @@
         <v>270</v>
       </c>
       <c r="J25" s="9" t="s">
+        <v>705</v>
+      </c>
+      <c r="K25" s="9" t="s">
         <v>706</v>
-      </c>
-      <c r="K25" s="9" t="s">
-        <v>707</v>
       </c>
       <c r="L25" s="9" t="s">
         <v>461</v>
       </c>
       <c r="M25" s="9"/>
       <c r="N25" s="9" t="s">
+        <v>707</v>
+      </c>
+      <c r="O25" s="9" t="s">
         <v>708</v>
-      </c>
-      <c r="O25" s="9" t="s">
-        <v>709</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5401,7 +5492,7 @@
         <v>427</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>261</v>
@@ -5421,15 +5512,15 @@
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
       <c r="K26" s="9" t="s">
+        <v>875</v>
+      </c>
+      <c r="L26" s="9" t="s">
         <v>876</v>
-      </c>
-      <c r="L26" s="9" t="s">
-        <v>877</v>
       </c>
       <c r="M26" s="9"/>
       <c r="N26" s="9"/>
       <c r="O26" s="9" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5440,7 +5531,7 @@
         <v>272</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>261</v>
@@ -5461,7 +5552,7 @@
         <v>273</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="K27" s="9" t="s">
         <v>455</v>
@@ -5473,10 +5564,10 @@
         <v>0</v>
       </c>
       <c r="N27" s="9" t="s">
+        <v>710</v>
+      </c>
+      <c r="O27" s="9" t="s">
         <v>711</v>
-      </c>
-      <c r="O27" s="9" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5487,7 +5578,7 @@
         <v>275</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>261</v>
@@ -5508,10 +5599,10 @@
         <v>276</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="K28" s="9" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="L28" s="9" t="s">
         <v>471</v>
@@ -5520,10 +5611,10 @@
         <v>0</v>
       </c>
       <c r="N28" s="9" t="s">
+        <v>713</v>
+      </c>
+      <c r="O28" s="9" t="s">
         <v>714</v>
-      </c>
-      <c r="O28" s="9" t="s">
-        <v>715</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5534,7 +5625,7 @@
         <v>278</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>261</v>
@@ -5555,10 +5646,10 @@
         <v>279</v>
       </c>
       <c r="J29" s="9" t="s">
+        <v>715</v>
+      </c>
+      <c r="K29" s="9" t="s">
         <v>716</v>
-      </c>
-      <c r="K29" s="9" t="s">
-        <v>717</v>
       </c>
       <c r="L29" s="9" t="s">
         <v>461</v>
@@ -5567,10 +5658,10 @@
         <v>0</v>
       </c>
       <c r="N29" s="9" t="s">
+        <v>717</v>
+      </c>
+      <c r="O29" s="9" t="s">
         <v>718</v>
-      </c>
-      <c r="O29" s="9" t="s">
-        <v>719</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5581,7 +5672,7 @@
         <v>281</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>261</v>
@@ -5602,20 +5693,20 @@
         <v>282</v>
       </c>
       <c r="J30" s="9" t="s">
+        <v>719</v>
+      </c>
+      <c r="K30" s="9" t="s">
         <v>720</v>
       </c>
-      <c r="K30" s="9" t="s">
+      <c r="L30" s="9" t="s">
         <v>721</v>
-      </c>
-      <c r="L30" s="9" t="s">
-        <v>722</v>
       </c>
       <c r="M30" s="9"/>
       <c r="N30" s="9" t="s">
+        <v>722</v>
+      </c>
+      <c r="O30" s="9" t="s">
         <v>723</v>
-      </c>
-      <c r="O30" s="9" t="s">
-        <v>724</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5626,7 +5717,7 @@
         <v>284</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>261</v>
@@ -5647,20 +5738,20 @@
         <v>285</v>
       </c>
       <c r="J31" s="9" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="K31" s="9" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="L31" s="9" t="s">
         <v>456</v>
       </c>
       <c r="M31" s="9"/>
       <c r="N31" s="9" t="s">
+        <v>725</v>
+      </c>
+      <c r="O31" s="9" t="s">
         <v>726</v>
-      </c>
-      <c r="O31" s="9" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5671,13 +5762,13 @@
         <v>178</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>179</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="4" t="s">
@@ -5710,7 +5801,7 @@
         <v>441</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>179</v>
@@ -5733,10 +5824,10 @@
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
       <c r="N33" s="9" t="s">
+        <v>892</v>
+      </c>
+      <c r="O33" s="9" t="s">
         <v>893</v>
-      </c>
-      <c r="O33" s="9" t="s">
-        <v>894</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5747,7 +5838,7 @@
         <v>180</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>179</v>
@@ -5792,7 +5883,7 @@
         <v>186</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>179</v>
@@ -5837,7 +5928,7 @@
         <v>443</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>179</v>
@@ -5859,17 +5950,17 @@
       </c>
       <c r="J36" s="9"/>
       <c r="K36" s="9" t="s">
+        <v>894</v>
+      </c>
+      <c r="L36" s="9" t="s">
         <v>895</v>
-      </c>
-      <c r="L36" s="9" t="s">
-        <v>896</v>
       </c>
       <c r="M36" s="9"/>
       <c r="N36" s="9" t="s">
+        <v>896</v>
+      </c>
+      <c r="O36" s="9" t="s">
         <v>897</v>
-      </c>
-      <c r="O36" s="9" t="s">
-        <v>898</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -5880,7 +5971,7 @@
         <v>189</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>179</v>
@@ -5927,7 +6018,7 @@
         <v>192</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D38" s="9" t="s">
         <v>179</v>
@@ -5974,7 +6065,7 @@
         <v>195</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D39" s="9" t="s">
         <v>179</v>
@@ -6019,7 +6110,7 @@
         <v>198</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D40" s="9" t="s">
         <v>179</v>
@@ -6066,13 +6157,13 @@
         <v>45</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>46</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F41" s="5"/>
       <c r="G41" s="4" t="s">
@@ -6101,7 +6192,7 @@
         <v>48</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D42" s="9" t="s">
         <v>46</v>
@@ -6146,13 +6237,13 @@
         <v>116</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>117</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F43" s="5"/>
       <c r="G43" s="4" t="s">
@@ -6185,7 +6276,7 @@
         <v>119</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D44" s="9" t="s">
         <v>117</v>
@@ -6232,7 +6323,7 @@
         <v>125</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D45" s="9" t="s">
         <v>117</v>
@@ -6277,7 +6368,7 @@
         <v>122</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>117</v>
@@ -6322,7 +6413,7 @@
         <v>128</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D47" s="9" t="s">
         <v>117</v>
@@ -6367,13 +6458,13 @@
         <v>160</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>161</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="4" t="s">
@@ -6398,7 +6489,7 @@
         <v>163</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D49" s="9" t="s">
         <v>161</v>
@@ -6443,7 +6534,7 @@
         <v>166</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D50" s="9" t="s">
         <v>161</v>
@@ -6488,7 +6579,7 @@
         <v>169</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D51" s="9" t="s">
         <v>161</v>
@@ -6533,13 +6624,13 @@
         <v>327</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>328</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F52" s="5"/>
       <c r="G52" s="4" t="s">
@@ -6564,7 +6655,7 @@
         <v>330</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D53" s="9" t="s">
         <v>328</v>
@@ -6585,10 +6676,10 @@
         <v>331</v>
       </c>
       <c r="J53" s="9" t="s">
+        <v>769</v>
+      </c>
+      <c r="K53" s="9" t="s">
         <v>770</v>
-      </c>
-      <c r="K53" s="9" t="s">
-        <v>771</v>
       </c>
       <c r="L53" s="9" t="s">
         <v>461</v>
@@ -6598,7 +6689,7 @@
         <v>0</v>
       </c>
       <c r="O53" s="9" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="54" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6609,7 +6700,7 @@
         <v>421</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D54" s="9" t="s">
         <v>328</v>
@@ -6629,17 +6720,17 @@
       <c r="I54" s="9"/>
       <c r="J54" s="9"/>
       <c r="K54" s="9" t="s">
+        <v>866</v>
+      </c>
+      <c r="L54" s="9" t="s">
         <v>867</v>
-      </c>
-      <c r="L54" s="9" t="s">
-        <v>868</v>
       </c>
       <c r="M54" s="9"/>
       <c r="N54" s="9" t="s">
+        <v>868</v>
+      </c>
+      <c r="O54" s="9" t="s">
         <v>869</v>
-      </c>
-      <c r="O54" s="9" t="s">
-        <v>870</v>
       </c>
     </row>
     <row r="55" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6650,7 +6741,7 @@
         <v>424</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D55" s="9" t="s">
         <v>328</v>
@@ -6669,20 +6760,20 @@
       </c>
       <c r="I55" s="9"/>
       <c r="J55" s="9" t="s">
+        <v>870</v>
+      </c>
+      <c r="K55" s="9" t="s">
         <v>871</v>
       </c>
-      <c r="K55" s="9" t="s">
+      <c r="L55" s="9" t="s">
         <v>872</v>
-      </c>
-      <c r="L55" s="9" t="s">
-        <v>873</v>
       </c>
       <c r="M55" s="9"/>
       <c r="N55" s="9" t="s">
+        <v>873</v>
+      </c>
+      <c r="O55" s="9" t="s">
         <v>874</v>
-      </c>
-      <c r="O55" s="9" t="s">
-        <v>875</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6693,7 +6784,7 @@
         <v>357</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D56" s="9" t="s">
         <v>328</v>
@@ -6714,20 +6805,20 @@
         <v>358</v>
       </c>
       <c r="J56" s="9" t="s">
+        <v>803</v>
+      </c>
+      <c r="K56" s="9" t="s">
         <v>804</v>
-      </c>
-      <c r="K56" s="9" t="s">
-        <v>805</v>
       </c>
       <c r="L56" s="9" t="s">
         <v>461</v>
       </c>
       <c r="M56" s="9"/>
       <c r="N56" s="9" t="s">
+        <v>805</v>
+      </c>
+      <c r="O56" s="9" t="s">
         <v>806</v>
-      </c>
-      <c r="O56" s="9" t="s">
-        <v>807</v>
       </c>
     </row>
     <row r="57" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6738,7 +6829,7 @@
         <v>378</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>328</v>
@@ -6759,10 +6850,10 @@
         <v>379</v>
       </c>
       <c r="J57" s="9" t="s">
+        <v>831</v>
+      </c>
+      <c r="K57" s="9" t="s">
         <v>832</v>
-      </c>
-      <c r="K57" s="9" t="s">
-        <v>833</v>
       </c>
       <c r="L57" s="9" t="s">
         <v>461</v>
@@ -6770,7 +6861,7 @@
       <c r="M57" s="9"/>
       <c r="N57" s="9"/>
       <c r="O57" s="9" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="58" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6781,7 +6872,7 @@
         <v>336</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D58" s="9" t="s">
         <v>328</v>
@@ -6802,20 +6893,20 @@
         <v>337</v>
       </c>
       <c r="J58" s="9" t="s">
+        <v>776</v>
+      </c>
+      <c r="K58" s="9" t="s">
         <v>777</v>
       </c>
-      <c r="K58" s="9" t="s">
+      <c r="L58" s="9" t="s">
         <v>778</v>
-      </c>
-      <c r="L58" s="9" t="s">
-        <v>779</v>
       </c>
       <c r="M58" s="9"/>
       <c r="N58" s="9" t="s">
+        <v>779</v>
+      </c>
+      <c r="O58" s="9" t="s">
         <v>780</v>
-      </c>
-      <c r="O58" s="9" t="s">
-        <v>781</v>
       </c>
     </row>
     <row r="59" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6826,7 +6917,7 @@
         <v>339</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>328</v>
@@ -6847,7 +6938,7 @@
         <v>340</v>
       </c>
       <c r="J59" s="9" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="K59" s="9" t="s">
         <v>592</v>
@@ -6859,10 +6950,10 @@
         <v>0</v>
       </c>
       <c r="N59" s="9" t="s">
+        <v>782</v>
+      </c>
+      <c r="O59" s="9" t="s">
         <v>783</v>
-      </c>
-      <c r="O59" s="9" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="60" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6873,7 +6964,7 @@
         <v>342</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D60" s="9" t="s">
         <v>328</v>
@@ -6894,7 +6985,7 @@
         <v>343</v>
       </c>
       <c r="J60" s="9" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="K60" s="9" t="s">
         <v>666</v>
@@ -6906,10 +6997,10 @@
         <v>0</v>
       </c>
       <c r="N60" s="9" t="s">
+        <v>785</v>
+      </c>
+      <c r="O60" s="9" t="s">
         <v>786</v>
-      </c>
-      <c r="O60" s="9" t="s">
-        <v>787</v>
       </c>
     </row>
     <row r="61" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6920,7 +7011,7 @@
         <v>369</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D61" s="9" t="s">
         <v>328</v>
@@ -6941,20 +7032,20 @@
         <v>370</v>
       </c>
       <c r="J61" s="9" t="s">
+        <v>818</v>
+      </c>
+      <c r="K61" s="9" t="s">
         <v>819</v>
-      </c>
-      <c r="K61" s="9" t="s">
-        <v>820</v>
       </c>
       <c r="L61" s="9" t="s">
         <v>461</v>
       </c>
       <c r="M61" s="9"/>
       <c r="N61" s="9" t="s">
+        <v>820</v>
+      </c>
+      <c r="O61" s="9" t="s">
         <v>821</v>
-      </c>
-      <c r="O61" s="9" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="62" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6965,7 +7056,7 @@
         <v>345</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D62" s="9" t="s">
         <v>328</v>
@@ -6986,20 +7077,20 @@
         <v>346</v>
       </c>
       <c r="J62" s="9" t="s">
+        <v>787</v>
+      </c>
+      <c r="K62" s="9" t="s">
         <v>788</v>
-      </c>
-      <c r="K62" s="9" t="s">
-        <v>789</v>
       </c>
       <c r="L62" s="9" t="s">
         <v>456</v>
       </c>
       <c r="M62" s="9"/>
       <c r="N62" s="9" t="s">
+        <v>789</v>
+      </c>
+      <c r="O62" s="9" t="s">
         <v>790</v>
-      </c>
-      <c r="O62" s="9" t="s">
-        <v>791</v>
       </c>
     </row>
     <row r="63" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7010,7 +7101,7 @@
         <v>348</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D63" s="9" t="s">
         <v>328</v>
@@ -7031,20 +7122,20 @@
         <v>349</v>
       </c>
       <c r="J63" s="9" t="s">
+        <v>791</v>
+      </c>
+      <c r="K63" s="9" t="s">
         <v>792</v>
-      </c>
-      <c r="K63" s="9" t="s">
-        <v>793</v>
       </c>
       <c r="L63" s="9" t="s">
         <v>456</v>
       </c>
       <c r="M63" s="9"/>
       <c r="N63" s="9" t="s">
+        <v>793</v>
+      </c>
+      <c r="O63" s="9" t="s">
         <v>794</v>
-      </c>
-      <c r="O63" s="9" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="64" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7055,7 +7146,7 @@
         <v>351</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D64" s="9" t="s">
         <v>328</v>
@@ -7076,20 +7167,20 @@
         <v>352</v>
       </c>
       <c r="J64" s="9" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="K64" s="9" t="s">
         <v>455</v>
       </c>
       <c r="L64" s="9" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="M64" s="9"/>
       <c r="N64" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="O64" s="9" t="s">
         <v>798</v>
-      </c>
-      <c r="O64" s="9" t="s">
-        <v>799</v>
       </c>
     </row>
     <row r="65" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7100,7 +7191,7 @@
         <v>354</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D65" s="9" t="s">
         <v>328</v>
@@ -7121,20 +7212,20 @@
         <v>355</v>
       </c>
       <c r="J65" s="9" t="s">
+        <v>799</v>
+      </c>
+      <c r="K65" s="9" t="s">
         <v>800</v>
-      </c>
-      <c r="K65" s="9" t="s">
-        <v>801</v>
       </c>
       <c r="L65" s="9" t="s">
         <v>456</v>
       </c>
       <c r="M65" s="9"/>
       <c r="N65" s="9" t="s">
+        <v>801</v>
+      </c>
+      <c r="O65" s="9" t="s">
         <v>802</v>
-      </c>
-      <c r="O65" s="9" t="s">
-        <v>803</v>
       </c>
     </row>
     <row r="66" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7145,7 +7236,7 @@
         <v>363</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D66" s="9" t="s">
         <v>328</v>
@@ -7166,10 +7257,10 @@
         <v>364</v>
       </c>
       <c r="J66" s="9" t="s">
+        <v>810</v>
+      </c>
+      <c r="K66" s="9" t="s">
         <v>811</v>
-      </c>
-      <c r="K66" s="9" t="s">
-        <v>812</v>
       </c>
       <c r="L66" s="9" t="s">
         <v>461</v>
@@ -7178,10 +7269,10 @@
         <v>0</v>
       </c>
       <c r="N66" s="9" t="s">
+        <v>812</v>
+      </c>
+      <c r="O66" s="9" t="s">
         <v>813</v>
-      </c>
-      <c r="O66" s="9" t="s">
-        <v>814</v>
       </c>
     </row>
     <row r="67" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7192,7 +7283,7 @@
         <v>429</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D67" s="9" t="s">
         <v>328</v>
@@ -7214,17 +7305,17 @@
       </c>
       <c r="J67" s="9"/>
       <c r="K67" s="9" t="s">
+        <v>878</v>
+      </c>
+      <c r="L67" s="9" t="s">
         <v>879</v>
-      </c>
-      <c r="L67" s="9" t="s">
-        <v>880</v>
       </c>
       <c r="M67" s="9"/>
       <c r="N67" s="9" t="s">
+        <v>880</v>
+      </c>
+      <c r="O67" s="9" t="s">
         <v>881</v>
-      </c>
-      <c r="O67" s="9" t="s">
-        <v>882</v>
       </c>
     </row>
     <row r="68" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7235,7 +7326,7 @@
         <v>360</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D68" s="9" t="s">
         <v>328</v>
@@ -7256,20 +7347,20 @@
         <v>361</v>
       </c>
       <c r="J68" s="9" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="K68" s="9" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="L68" s="9" t="s">
         <v>461</v>
       </c>
       <c r="M68" s="9"/>
       <c r="N68" s="9" t="s">
+        <v>808</v>
+      </c>
+      <c r="O68" s="9" t="s">
         <v>809</v>
-      </c>
-      <c r="O68" s="9" t="s">
-        <v>810</v>
       </c>
     </row>
     <row r="69" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7280,13 +7371,13 @@
         <v>72</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>73</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F69" s="5"/>
       <c r="G69" s="4" t="s">
@@ -7311,7 +7402,7 @@
         <v>75</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D70" s="9" t="s">
         <v>73</v>
@@ -7356,7 +7447,7 @@
         <v>78</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D71" s="9" t="s">
         <v>73</v>
@@ -7401,7 +7492,7 @@
         <v>83</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D72" s="9" t="s">
         <v>73</v>
@@ -7446,7 +7537,7 @@
         <v>80</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D73" s="9" t="s">
         <v>73</v>
@@ -7491,7 +7582,7 @@
         <v>86</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D74" s="9" t="s">
         <v>73</v>
@@ -7566,7 +7657,7 @@
         <v>566</v>
       </c>
       <c r="O75" s="9" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="76" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7583,7 +7674,7 @@
         <v>135</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F76" s="5"/>
       <c r="G76" s="4" t="s">
@@ -7804,7 +7895,7 @@
         <v>52</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F81" s="5"/>
       <c r="G81" s="4" t="s">
@@ -7831,13 +7922,13 @@
         <v>89</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>90</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F82" s="5"/>
       <c r="G82" s="4" t="s">
@@ -7864,7 +7955,7 @@
         <v>92</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>90</v>
@@ -7909,7 +8000,7 @@
         <v>183</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D84" s="9" t="s">
         <v>179</v>
@@ -7954,7 +8045,7 @@
         <v>438</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D85" s="9" t="s">
         <v>179</v>
@@ -7974,15 +8065,15 @@
       <c r="I85" s="9"/>
       <c r="J85" s="9"/>
       <c r="K85" s="9" t="s">
+        <v>889</v>
+      </c>
+      <c r="L85" s="9" t="s">
         <v>890</v>
-      </c>
-      <c r="L85" s="9" t="s">
-        <v>891</v>
       </c>
       <c r="M85" s="9"/>
       <c r="N85" s="9"/>
       <c r="O85" s="9" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="86" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -7993,7 +8084,7 @@
         <v>201</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D86" s="9" t="s">
         <v>179</v>
@@ -8038,7 +8129,7 @@
         <v>205</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D87" s="9" t="s">
         <v>179</v>
@@ -8083,7 +8174,7 @@
         <v>445</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D88" s="9" t="s">
         <v>179</v>
@@ -8103,7 +8194,7 @@
       <c r="I88" s="9"/>
       <c r="J88" s="9"/>
       <c r="K88" s="9" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="L88" s="9" t="s">
         <v>538</v>
@@ -8111,7 +8202,7 @@
       <c r="M88" s="9"/>
       <c r="N88" s="9"/>
       <c r="O88" s="9" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="89" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8122,7 +8213,7 @@
         <v>212</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D89" s="9" t="s">
         <v>179</v>
@@ -8161,7 +8252,7 @@
         <v>215</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D90" s="9" t="s">
         <v>179</v>
@@ -8200,7 +8291,7 @@
         <v>209</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D91" s="9" t="s">
         <v>179</v>
@@ -8245,7 +8336,7 @@
         <v>218</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D92" s="9" t="s">
         <v>179</v>
@@ -8288,7 +8379,7 @@
         <v>222</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D93" s="9" t="s">
         <v>179</v>
@@ -8327,13 +8418,13 @@
         <v>317</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>318</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F94" s="5"/>
       <c r="G94" s="4" t="s">
@@ -8350,7 +8441,7 @@
         <v>315</v>
       </c>
       <c r="N94" s="4" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="O94" s="4"/>
     </row>
@@ -8362,7 +8453,7 @@
         <v>320</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D95" s="9" t="s">
         <v>318</v>
@@ -8383,20 +8474,20 @@
         <v>321</v>
       </c>
       <c r="J95" s="9" t="s">
+        <v>760</v>
+      </c>
+      <c r="K95" s="9" t="s">
         <v>761</v>
-      </c>
-      <c r="K95" s="9" t="s">
-        <v>762</v>
       </c>
       <c r="L95" s="9" t="s">
         <v>456</v>
       </c>
       <c r="M95" s="9"/>
       <c r="N95" s="9" t="s">
+        <v>762</v>
+      </c>
+      <c r="O95" s="9" t="s">
         <v>763</v>
-      </c>
-      <c r="O95" s="9" t="s">
-        <v>764</v>
       </c>
     </row>
     <row r="96" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8407,7 +8498,7 @@
         <v>324</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D96" s="9" t="s">
         <v>318</v>
@@ -8428,20 +8519,20 @@
         <v>325</v>
       </c>
       <c r="J96" s="9" t="s">
+        <v>764</v>
+      </c>
+      <c r="K96" s="9" t="s">
         <v>765</v>
-      </c>
-      <c r="K96" s="9" t="s">
-        <v>766</v>
       </c>
       <c r="L96" s="9" t="s">
         <v>461</v>
       </c>
       <c r="M96" s="9"/>
       <c r="N96" s="9" t="s">
+        <v>766</v>
+      </c>
+      <c r="O96" s="9" t="s">
         <v>767</v>
-      </c>
-      <c r="O96" s="9" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="97" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8452,7 +8543,7 @@
         <v>411</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D97" s="9" t="s">
         <v>318</v>
@@ -8474,17 +8565,17 @@
       </c>
       <c r="J97" s="9"/>
       <c r="K97" s="9" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="L97" s="9" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="M97" s="9"/>
       <c r="N97" s="9" t="s">
+        <v>859</v>
+      </c>
+      <c r="O97" s="9" t="s">
         <v>860</v>
-      </c>
-      <c r="O97" s="9" t="s">
-        <v>861</v>
       </c>
     </row>
     <row r="98" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8495,13 +8586,13 @@
         <v>150</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>151</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F98" s="5"/>
       <c r="G98" s="4" t="s">
@@ -8526,13 +8617,13 @@
         <v>314</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>315</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F99" s="5"/>
       <c r="G99" s="4" t="s">
@@ -8550,7 +8641,7 @@
       </c>
       <c r="N99" s="4"/>
       <c r="O99" s="4" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="100" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8561,13 +8652,13 @@
         <v>95</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>96</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F100" s="5"/>
       <c r="G100" s="4" t="s">
@@ -8594,7 +8685,7 @@
         <v>98</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D101" s="9" t="s">
         <v>96</v>
@@ -8639,7 +8730,7 @@
         <v>101</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D102" s="9" t="s">
         <v>96</v>
@@ -8684,13 +8775,13 @@
         <v>131</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D103" s="4" t="s">
         <v>132</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F103" s="5"/>
       <c r="G103" s="4" t="s">
@@ -8721,13 +8812,13 @@
         <v>37</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D104" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E104" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F104" s="5"/>
       <c r="G104" s="4" t="s">
@@ -8754,7 +8845,7 @@
         <v>40</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D105" s="9" t="s">
         <v>38</v>
@@ -8799,13 +8890,13 @@
         <v>104</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D106" s="4" t="s">
         <v>105</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F106" s="5"/>
       <c r="G106" s="5"/>
@@ -8828,7 +8919,7 @@
         <v>112</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D107" s="9" t="s">
         <v>105</v>
@@ -8871,7 +8962,7 @@
         <v>106</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D108" s="9" t="s">
         <v>105</v>
@@ -8916,7 +9007,7 @@
         <v>109</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D109" s="9" t="s">
         <v>105</v>
@@ -8961,13 +9052,13 @@
         <v>407</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D110" s="4" t="s">
         <v>408</v>
       </c>
       <c r="E110" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F110" s="5"/>
       <c r="G110" s="4" t="s">
@@ -8992,7 +9083,7 @@
         <v>417</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D111" s="9" t="s">
         <v>408</v>
@@ -9017,14 +9108,14 @@
         <v>645</v>
       </c>
       <c r="L111" s="9" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="M111" s="9"/>
       <c r="N111" s="9" t="s">
+        <v>861</v>
+      </c>
+      <c r="O111" s="9" t="s">
         <v>862</v>
-      </c>
-      <c r="O111" s="9" t="s">
-        <v>863</v>
       </c>
     </row>
     <row r="112" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9035,7 +9126,7 @@
         <v>415</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D112" s="9" t="s">
         <v>408</v>
@@ -9064,10 +9155,10 @@
       </c>
       <c r="M112" s="9"/>
       <c r="N112" s="9" t="s">
+        <v>861</v>
+      </c>
+      <c r="O112" s="9" t="s">
         <v>862</v>
-      </c>
-      <c r="O112" s="9" t="s">
-        <v>863</v>
       </c>
     </row>
     <row r="113" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9078,7 +9169,7 @@
         <v>419</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D113" s="9" t="s">
         <v>408</v>
@@ -9100,17 +9191,17 @@
       </c>
       <c r="J113" s="9"/>
       <c r="K113" s="9" t="s">
+        <v>734</v>
+      </c>
+      <c r="L113" s="9" t="s">
         <v>735</v>
-      </c>
-      <c r="L113" s="9" t="s">
-        <v>736</v>
       </c>
       <c r="M113" s="9"/>
       <c r="N113" s="9" t="s">
+        <v>864</v>
+      </c>
+      <c r="O113" s="9" t="s">
         <v>865</v>
-      </c>
-      <c r="O113" s="9" t="s">
-        <v>866</v>
       </c>
     </row>
     <row r="114" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9121,13 +9212,13 @@
         <v>381</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D114" s="4" t="s">
         <v>382</v>
       </c>
       <c r="E114" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F114" s="5"/>
       <c r="G114" s="4" t="s">
@@ -9152,7 +9243,7 @@
         <v>387</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D115" s="9" t="s">
         <v>382</v>
@@ -9173,20 +9264,20 @@
         <v>388</v>
       </c>
       <c r="J115" s="9" t="s">
+        <v>838</v>
+      </c>
+      <c r="K115" s="9" t="s">
         <v>839</v>
-      </c>
-      <c r="K115" s="9" t="s">
-        <v>840</v>
       </c>
       <c r="L115" s="9" t="s">
         <v>461</v>
       </c>
       <c r="M115" s="9"/>
       <c r="N115" s="9" t="s">
+        <v>840</v>
+      </c>
+      <c r="O115" s="9" t="s">
         <v>841</v>
-      </c>
-      <c r="O115" s="9" t="s">
-        <v>842</v>
       </c>
     </row>
     <row r="116" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9197,7 +9288,7 @@
         <v>385</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D116" s="9" t="s">
         <v>382</v>
@@ -9218,20 +9309,20 @@
         <v>386</v>
       </c>
       <c r="J116" s="9" t="s">
+        <v>834</v>
+      </c>
+      <c r="K116" s="9" t="s">
         <v>835</v>
-      </c>
-      <c r="K116" s="9" t="s">
-        <v>836</v>
       </c>
       <c r="L116" s="9" t="s">
         <v>461</v>
       </c>
       <c r="M116" s="9"/>
       <c r="N116" s="9" t="s">
+        <v>836</v>
+      </c>
+      <c r="O116" s="9" t="s">
         <v>837</v>
-      </c>
-      <c r="O116" s="9" t="s">
-        <v>838</v>
       </c>
     </row>
     <row r="117" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9242,7 +9333,7 @@
         <v>390</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D117" s="9" t="s">
         <v>382</v>
@@ -9263,20 +9354,20 @@
         <v>391</v>
       </c>
       <c r="J117" s="9" t="s">
+        <v>842</v>
+      </c>
+      <c r="K117" s="9" t="s">
         <v>843</v>
-      </c>
-      <c r="K117" s="9" t="s">
-        <v>844</v>
       </c>
       <c r="L117" s="9" t="s">
         <v>604</v>
       </c>
       <c r="M117" s="9"/>
       <c r="N117" s="9" t="s">
+        <v>844</v>
+      </c>
+      <c r="O117" s="9" t="s">
         <v>845</v>
-      </c>
-      <c r="O117" s="9" t="s">
-        <v>846</v>
       </c>
     </row>
     <row r="118" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9287,13 +9378,13 @@
         <v>393</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D118" s="4" t="s">
         <v>394</v>
       </c>
       <c r="E118" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F118" s="5"/>
       <c r="G118" s="4" t="s">
@@ -9318,7 +9409,7 @@
         <v>396</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D119" s="9" t="s">
         <v>394</v>
@@ -9339,7 +9430,7 @@
         <v>397</v>
       </c>
       <c r="J119" s="9" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="K119" s="9" t="s">
         <v>666</v>
@@ -9349,10 +9440,10 @@
       </c>
       <c r="M119" s="9"/>
       <c r="N119" s="9" t="s">
+        <v>847</v>
+      </c>
+      <c r="O119" s="9" t="s">
         <v>848</v>
-      </c>
-      <c r="O119" s="9" t="s">
-        <v>849</v>
       </c>
     </row>
     <row r="120" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9363,7 +9454,7 @@
         <v>405</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D120" s="9" t="s">
         <v>394</v>
@@ -9385,17 +9476,17 @@
       </c>
       <c r="J120" s="9"/>
       <c r="K120" s="9" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="L120" s="9" t="s">
         <v>456</v>
       </c>
       <c r="M120" s="9"/>
       <c r="N120" s="9" t="s">
+        <v>856</v>
+      </c>
+      <c r="O120" s="9" t="s">
         <v>857</v>
-      </c>
-      <c r="O120" s="9" t="s">
-        <v>858</v>
       </c>
     </row>
     <row r="121" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9406,7 +9497,7 @@
         <v>399</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D121" s="9" t="s">
         <v>394</v>
@@ -9427,7 +9518,7 @@
         <v>400</v>
       </c>
       <c r="J121" s="9" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="K121" s="9" t="s">
         <v>455</v>
@@ -9437,10 +9528,10 @@
       </c>
       <c r="M121" s="9"/>
       <c r="N121" s="9" t="s">
+        <v>850</v>
+      </c>
+      <c r="O121" s="9" t="s">
         <v>851</v>
-      </c>
-      <c r="O121" s="9" t="s">
-        <v>852</v>
       </c>
     </row>
     <row r="122" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9451,7 +9542,7 @@
         <v>402</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D122" s="9" t="s">
         <v>394</v>
@@ -9472,7 +9563,7 @@
         <v>403</v>
       </c>
       <c r="J122" s="9" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="K122" s="9" t="s">
         <v>455</v>
@@ -9482,10 +9573,10 @@
       </c>
       <c r="M122" s="9"/>
       <c r="N122" s="9" t="s">
+        <v>853</v>
+      </c>
+      <c r="O122" s="9" t="s">
         <v>854</v>
-      </c>
-      <c r="O122" s="9" t="s">
-        <v>855</v>
       </c>
     </row>
     <row r="123" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9496,13 +9587,13 @@
         <v>296</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D123" s="4" t="s">
         <v>297</v>
       </c>
       <c r="E123" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F123" s="5"/>
       <c r="G123" s="4" t="s">
@@ -9514,14 +9605,14 @@
       </c>
       <c r="J123" s="4"/>
       <c r="K123" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="L123" s="4" t="s">
         <v>735</v>
-      </c>
-      <c r="L123" s="4" t="s">
-        <v>736</v>
       </c>
       <c r="M123" s="4"/>
       <c r="N123" s="4" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="O123" s="4"/>
     </row>
@@ -9533,7 +9624,7 @@
         <v>299</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D124" s="9" t="s">
         <v>297</v>
@@ -9554,20 +9645,20 @@
         <v>300</v>
       </c>
       <c r="J124" s="9" t="s">
+        <v>737</v>
+      </c>
+      <c r="K124" s="9" t="s">
         <v>738</v>
       </c>
-      <c r="K124" s="9" t="s">
+      <c r="L124" s="9" t="s">
         <v>739</v>
-      </c>
-      <c r="L124" s="9" t="s">
-        <v>740</v>
       </c>
       <c r="M124" s="9"/>
       <c r="N124" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="O124" s="9" t="s">
         <v>741</v>
-      </c>
-      <c r="O124" s="9" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="125" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9578,7 +9669,7 @@
         <v>302</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D125" s="9" t="s">
         <v>297</v>
@@ -9599,20 +9690,20 @@
         <v>303</v>
       </c>
       <c r="J125" s="9" t="s">
+        <v>742</v>
+      </c>
+      <c r="K125" s="9" t="s">
         <v>743</v>
       </c>
-      <c r="K125" s="9" t="s">
-        <v>744</v>
-      </c>
       <c r="L125" s="9" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="M125" s="9"/>
       <c r="N125" s="9" t="s">
+        <v>744</v>
+      </c>
+      <c r="O125" s="9" t="s">
         <v>745</v>
-      </c>
-      <c r="O125" s="9" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="126" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9623,7 +9714,7 @@
         <v>305</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D126" s="9" t="s">
         <v>297</v>
@@ -9644,20 +9735,20 @@
         <v>306</v>
       </c>
       <c r="J126" s="9" t="s">
+        <v>746</v>
+      </c>
+      <c r="K126" s="9" t="s">
         <v>747</v>
       </c>
-      <c r="K126" s="9" t="s">
-        <v>748</v>
-      </c>
       <c r="L126" s="9" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="M126" s="9"/>
       <c r="N126" s="9" t="s">
+        <v>748</v>
+      </c>
+      <c r="O126" s="9" t="s">
         <v>749</v>
-      </c>
-      <c r="O126" s="9" t="s">
-        <v>750</v>
       </c>
     </row>
     <row r="127" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9668,7 +9759,7 @@
         <v>308</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D127" s="9" t="s">
         <v>297</v>
@@ -9689,20 +9780,20 @@
         <v>309</v>
       </c>
       <c r="J127" s="9" t="s">
+        <v>750</v>
+      </c>
+      <c r="K127" s="9" t="s">
         <v>751</v>
       </c>
-      <c r="K127" s="9" t="s">
-        <v>752</v>
-      </c>
       <c r="L127" s="9" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="M127" s="9"/>
       <c r="N127" s="9" t="s">
+        <v>752</v>
+      </c>
+      <c r="O127" s="9" t="s">
         <v>753</v>
-      </c>
-      <c r="O127" s="9" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="128" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9713,7 +9804,7 @@
         <v>311</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D128" s="9" t="s">
         <v>297</v>
@@ -9734,20 +9825,20 @@
         <v>312</v>
       </c>
       <c r="J128" s="9" t="s">
+        <v>754</v>
+      </c>
+      <c r="K128" s="9" t="s">
         <v>755</v>
-      </c>
-      <c r="K128" s="9" t="s">
-        <v>756</v>
       </c>
       <c r="L128" s="9" t="s">
         <v>461</v>
       </c>
       <c r="M128" s="9"/>
       <c r="N128" s="9" t="s">
+        <v>756</v>
+      </c>
+      <c r="O128" s="9" t="s">
         <v>757</v>
-      </c>
-      <c r="O128" s="9" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="129" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9758,13 +9849,13 @@
         <v>30</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D129" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E129" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F129" s="5"/>
       <c r="G129" s="4" t="s">
@@ -9791,7 +9882,7 @@
         <v>33</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D130" s="9" t="s">
         <v>31</v>
@@ -9836,13 +9927,13 @@
         <v>21</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D131" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E131" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F131" s="5"/>
       <c r="G131" s="4" t="s">
@@ -9869,7 +9960,7 @@
         <v>24</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D132" s="9" t="s">
         <v>22</v>
@@ -9914,7 +10005,7 @@
         <v>27</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D133" s="9" t="s">
         <v>22</v>
@@ -10049,7 +10140,7 @@
         <v>68</v>
       </c>
       <c r="E136" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F136" s="5"/>
       <c r="G136" s="5"/>
@@ -10093,20 +10184,20 @@
         <v>334</v>
       </c>
       <c r="J137" s="9" t="s">
+        <v>772</v>
+      </c>
+      <c r="K137" s="9" t="s">
         <v>773</v>
-      </c>
-      <c r="K137" s="9" t="s">
-        <v>774</v>
       </c>
       <c r="L137" s="9" t="s">
         <v>461</v>
       </c>
       <c r="M137" s="9"/>
       <c r="N137" s="9" t="s">
+        <v>774</v>
+      </c>
+      <c r="O137" s="9" t="s">
         <v>775</v>
-      </c>
-      <c r="O137" s="9" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="138" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10136,20 +10227,20 @@
         <v>367</v>
       </c>
       <c r="J138" s="9" t="s">
+        <v>814</v>
+      </c>
+      <c r="K138" s="9" t="s">
         <v>815</v>
-      </c>
-      <c r="K138" s="9" t="s">
-        <v>816</v>
       </c>
       <c r="L138" s="9" t="s">
         <v>461</v>
       </c>
       <c r="M138" s="9"/>
       <c r="N138" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="O138" s="9" t="s">
         <v>817</v>
-      </c>
-      <c r="O138" s="9" t="s">
-        <v>818</v>
       </c>
     </row>
     <row r="139" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10179,10 +10270,10 @@
         <v>373</v>
       </c>
       <c r="J139" s="9" t="s">
+        <v>822</v>
+      </c>
+      <c r="K139" s="9" t="s">
         <v>823</v>
-      </c>
-      <c r="K139" s="9" t="s">
-        <v>824</v>
       </c>
       <c r="L139" s="9" t="s">
         <v>461</v>
@@ -10191,10 +10282,10 @@
         <v>0</v>
       </c>
       <c r="N139" s="9" t="s">
+        <v>824</v>
+      </c>
+      <c r="O139" s="9" t="s">
         <v>825</v>
-      </c>
-      <c r="O139" s="9" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="140" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10224,22 +10315,22 @@
         <v>376</v>
       </c>
       <c r="J140" s="9" t="s">
+        <v>826</v>
+      </c>
+      <c r="K140" s="9" t="s">
         <v>827</v>
       </c>
-      <c r="K140" s="9" t="s">
+      <c r="L140" s="9" t="s">
         <v>828</v>
-      </c>
-      <c r="L140" s="9" t="s">
-        <v>829</v>
       </c>
       <c r="M140" s="9" t="s">
         <v>0</v>
       </c>
       <c r="N140" s="9" t="s">
+        <v>829</v>
+      </c>
+      <c r="O140" s="9" t="s">
         <v>830</v>
-      </c>
-      <c r="O140" s="9" t="s">
-        <v>831</v>
       </c>
     </row>
     <row r="141" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10266,19 +10357,19 @@
       <c r="I141" s="9"/>
       <c r="J141" s="9"/>
       <c r="K141" s="9" t="s">
+        <v>882</v>
+      </c>
+      <c r="L141" s="9" t="s">
         <v>883</v>
       </c>
-      <c r="L141" s="9" t="s">
+      <c r="M141" s="9" t="s">
         <v>884</v>
-      </c>
-      <c r="M141" s="9" t="s">
-        <v>885</v>
       </c>
       <c r="N141" s="9" t="s">
         <v>483</v>
       </c>
       <c r="O141" s="9" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="142" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10551,7 +10642,7 @@
         <v>70</v>
       </c>
       <c r="E148" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F148" s="5"/>
       <c r="G148" s="4" t="s">
@@ -10569,6 +10660,31 @@
       </c>
       <c r="N148" s="4"/>
       <c r="O148" s="4"/>
+    </row>
+    <row r="149" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A149" s="15"/>
+      <c r="B149" s="16"/>
+      <c r="C149" s="16"/>
+      <c r="D149" s="17"/>
+      <c r="E149" s="18"/>
+      <c r="F149" s="18"/>
+      <c r="G149" s="18"/>
+      <c r="H149" s="18"/>
+      <c r="I149" s="17"/>
+      <c r="J149" s="17"/>
+      <c r="K149" s="19" t="s">
+        <v>919</v>
+      </c>
+      <c r="L149" s="19" t="s">
+        <v>916</v>
+      </c>
+      <c r="M149" s="19"/>
+      <c r="N149" s="19" t="s">
+        <v>918</v>
+      </c>
+      <c r="O149" s="19" t="s">
+        <v>917</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P149">

</xml_diff>

<commit_message>
Relaxed cardinality of CaseJudge and CaseProsecutingAttorney to allow add and delete in the same message
</commit_message>
<xml_diff>
--- a/schemas/CaseUpdates_iepd/artifacts/CaseInitiation_MappingSpreasheet - Case Updates.xlsx
+++ b/schemas/CaseUpdates_iepd/artifacts/CaseInitiation_MappingSpreasheet - Case Updates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\CaseUpdates_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0389824B-13A5-4CF8-A8F9-25A0FC4D33F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E8E34E-E038-43F6-AF90-639729BEC335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="944">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="945">
   <si>
     <t/>
   </si>
@@ -3442,6 +3442,9 @@
   </si>
   <si>
     <t>/nola:EntityUpdateExchange/j:Booking/j:BookingDocumentControlIdentification/IdentificationID</t>
+  </si>
+  <si>
+    <t>0..2</t>
   </si>
 </sst>
 </file>
@@ -4498,10 +4501,10 @@
   <dimension ref="A1:O152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="J124" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="H79" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J144" sqref="J144"/>
+      <selection pane="bottomRight" activeCell="H92" sqref="H92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -8327,7 +8330,7 @@
         <v>111</v>
       </c>
       <c r="H89" s="9" t="s">
-        <v>14</v>
+        <v>944</v>
       </c>
       <c r="I89" s="9" t="s">
         <v>213</v>
@@ -8405,7 +8408,7 @@
         <v>211</v>
       </c>
       <c r="H91" s="9" t="s">
-        <v>14</v>
+        <v>944</v>
       </c>
       <c r="I91" s="9" t="s">
         <v>210</v>

</xml_diff>

<commit_message>
Added CourtDispositionCode and CourtDispositionDate to CaseInitiation and CaseUpdates
</commit_message>
<xml_diff>
--- a/schemas/CaseUpdates_iepd/artifacts/CaseInitiation_MappingSpreasheet - Case Updates.xlsx
+++ b/schemas/CaseUpdates_iepd/artifacts/CaseInitiation_MappingSpreasheet - Case Updates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\CaseUpdates_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B439AD0-EB71-4E7C-B1C0-835F0894C938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D0602D-6189-40BD-99F5-1A01D8478FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4080" yWindow="-21720" windowWidth="51840" windowHeight="20760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4080" yWindow="-21720" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Case Initiation" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1954" uniqueCount="965">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1982" uniqueCount="978">
   <si>
     <t/>
   </si>
@@ -3512,12 +3512,57 @@
 /nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[5]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID
 /nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[6]/nola-ext:ChargeAugmentation/nola-ext:StatewideATNChargeSequenceID</t>
   </si>
+  <si>
+    <t>Charge Disposition Code</t>
+  </si>
+  <si>
+    <t>ChargeDisposiotion</t>
+  </si>
+  <si>
+    <t>ChargeDispositionCode</t>
+  </si>
+  <si>
+    <t>A value that describes the type of disposition.</t>
+  </si>
+  <si>
+    <t>[{"db": "AS400_JMS",	"table": "IMCHGD",	"fieldDesc": "DispositionCode",	"field": "ICDSPC"},
+{"db": "AS400_CDC_CMS",	"table": "CHRGLOG",	"fieldDesc": "DispositionCode",	"field": "CXDISP"},
+{"db": "AS400_CDC_CMS",	"table": "DISP",	"fieldDesc": "DispositionCode",	"field": "DP_DISPOSITION_CODE"},
+{"db": "AS400_CDC_CMS",	"table": "LookUp_IMCHGD_Dispositions",	"fieldDesc": "DispositionCode",	"field": "CODE"}]</t>
+  </si>
+  <si>
+    <t>nola-ext:ChargeDispositionCode</t>
+  </si>
+  <si>
+    <t>nola-ext:ChargeAugmentationType</t>
+  </si>
+  <si>
+    <t>j:CaseCharge/nola-ext:ChargeAugmentation/nola-ext:ChargeDispositionCode</t>
+  </si>
+  <si>
+    <t>/nola:CaseInitiationExchange/nc:CourtCase/j:CaseAugmentation/j:CaseCharge/nola-ext:ChargeAugmentation/ext:ChargeDispositionCode</t>
+  </si>
+  <si>
+    <t>ChargeDispositionDate</t>
+  </si>
+  <si>
+    <t>A date that a disposition was docketed in the court's system.</t>
+  </si>
+  <si>
+    <t>[{"db": "AS400_JMS",	"table": "IMCHGD",	"fieldDesc": "DispositionDate",	"field": "ICDSPD"},
+{"db": "AS400_CDC_CMS",	"table": "DISP",	"fieldDesc": "DispositionDate",	"field": "DPDATE"},
+{"db": "CASTNetDB",	"table": "PersonCharge",	"fieldDesc": "DispositionDate",	"field": "DispositionDate"},
+{"db": "MC",	"table": "Digicourt_Orleans.dbview.vw_CriminalCaseFileDetail", "fieldDesc": "DispositionDate", "field": "DISPOSITION_DATE"}]</t>
+  </si>
+  <si>
+    <t>/nola:CaseInitiationExchange/nc:CourtCase/j:CaseAugmentation/j:CaseCharge/j:ChargeDisposition/nc:DispositionDate/nc:Date</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -3535,6 +3580,12 @@
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -3570,7 +3621,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -3663,11 +3714,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3724,6 +3793,22 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4593,13 +4678,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O155"/>
+  <dimension ref="A1:V157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="1" topLeftCell="F127" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O155" sqref="O155"/>
+      <selection pane="bottomRight" activeCell="C157" sqref="C157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -10698,7 +10783,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="145" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A145" s="7" t="s">
         <v>12</v>
       </c>
@@ -10741,7 +10826,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="146" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A146" s="7" t="s">
         <v>12</v>
       </c>
@@ -10784,7 +10869,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="147" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A147" s="7" t="s">
         <v>12</v>
       </c>
@@ -10827,7 +10912,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="148" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A148" s="3" t="s">
         <v>8</v>
       </c>
@@ -10858,7 +10943,7 @@
       <c r="N148" s="4"/>
       <c r="O148" s="4"/>
     </row>
-    <row r="149" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A149" s="15" t="s">
         <v>12</v>
       </c>
@@ -10895,7 +10980,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="150" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A150" s="15" t="s">
         <v>12</v>
       </c>
@@ -10940,7 +11025,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="151" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A151" s="15" t="s">
         <v>12</v>
       </c>
@@ -10985,7 +11070,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="152" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A152" s="15" t="s">
         <v>12</v>
       </c>
@@ -11030,7 +11115,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="153" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A153" s="17" t="s">
         <v>12</v>
       </c>
@@ -11075,7 +11160,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="154" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A154" s="17" t="s">
         <v>12</v>
       </c>
@@ -11120,7 +11205,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="155" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A155" s="17" t="s">
         <v>12</v>
       </c>
@@ -11165,6 +11250,103 @@
       </c>
       <c r="O155" s="19" t="s">
         <v>961</v>
+      </c>
+    </row>
+    <row r="156" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A156" s="17" t="s">
+        <v>965</v>
+      </c>
+      <c r="B156" s="20">
+        <v>151</v>
+      </c>
+      <c r="C156" s="25" t="s">
+        <v>797</v>
+      </c>
+      <c r="D156" s="21" t="s">
+        <v>966</v>
+      </c>
+      <c r="E156" s="21" t="s">
+        <v>967</v>
+      </c>
+      <c r="F156" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G156" s="19" t="s">
+        <v>968</v>
+      </c>
+      <c r="H156" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I156" s="21" t="s">
+        <v>967</v>
+      </c>
+      <c r="J156" s="21" t="s">
+        <v>969</v>
+      </c>
+      <c r="K156" s="21" t="s">
+        <v>970</v>
+      </c>
+      <c r="L156" s="21" t="s">
+        <v>456</v>
+      </c>
+      <c r="M156" s="21" t="s">
+        <v>971</v>
+      </c>
+      <c r="N156" s="21" t="s">
+        <v>972</v>
+      </c>
+      <c r="O156" s="21" t="s">
+        <v>973</v>
+      </c>
+      <c r="T156" s="22"/>
+      <c r="U156" s="22"/>
+      <c r="V156" s="23"/>
+    </row>
+    <row r="157" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A157" s="17" t="s">
+        <v>965</v>
+      </c>
+      <c r="B157" s="20">
+        <v>152</v>
+      </c>
+      <c r="C157" s="25" t="s">
+        <v>797</v>
+      </c>
+      <c r="D157" s="21" t="s">
+        <v>966</v>
+      </c>
+      <c r="E157" s="21" t="s">
+        <v>974</v>
+      </c>
+      <c r="F157" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="G157" s="19" t="s">
+        <v>975</v>
+      </c>
+      <c r="H157" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I157" s="21" t="s">
+        <v>967</v>
+      </c>
+      <c r="J157" s="21" t="s">
+        <v>976</v>
+      </c>
+      <c r="K157" s="21" t="s">
+        <v>619</v>
+      </c>
+      <c r="L157" s="21" t="s">
+        <v>620</v>
+      </c>
+      <c r="M157" s="21" t="s">
+        <v>971</v>
+      </c>
+      <c r="N157" s="21" t="s">
+        <v>972</v>
+      </c>
+      <c r="O157" s="21" t="s">
+        <v>977</v>
       </c>
     </row>
   </sheetData>

</xml_diff>